<commit_message>
yess i am commiting skipping staging
</commit_message>
<xml_diff>
--- a/myexcel.xlsx
+++ b/myexcel.xlsx
@@ -11,7 +11,7 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -342,12 +342,40 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="B2">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="C3">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="D4">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="E5">
+        <v>567</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>